<commit_message>
ready to change reportng to allure report
</commit_message>
<xml_diff>
--- a/config/grammar.xlsx
+++ b/config/grammar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="28815" windowHeight="6405" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="28815" windowHeight="6405" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="rule" sheetId="1" r:id="rId1"/>
@@ -4503,11 +4503,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>百科欧洲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欧洲</t>
+    <t>百科大洋洲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大洋洲</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6629,7 +6629,7 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:D68"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8900,8 +8900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8963,8 +8963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>